<commit_message>
Pendiente correcciones para version final
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,243 +436,79 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">AAA040708SB8
-</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AAA060215LU2
-</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AAA060509UEA
-</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AAA061212Q15
-</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AAA080527HB7
-</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>AAA080627P15</t>
+          <t>AAA080527HB7</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELIAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TECNICOS Y DE PERSONAL ACADEMICO.', 'Vision': 'GARANTIZAR LA PROTECCION, CONSERVACION, RESTAURACION Y RECUPERACION, ASI COMO EL ESTUDIO, INVESTIGACION, DIFUSION DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRAFICOS Y MUSEOGRAFICOS QUE LO INTEGRAN.', 'Pagina web': 'www.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ALIAS CALLES ALVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMIREZ ESPAÑA, LIC. MARIA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '11', 'Plantilla voluntariado': '2', 'Monto total plantilla laboral': '296,282', 'Activo': '624,528', 'Pasivo': '6,055', 'Capital': '618,473', 'Gastos administracion': '710,777', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '1,826', 'Tipo de donante': 'Persona Física Extranjera'}, {'Especie ': '', 'Efectivo ': '489,406', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '924', 'Tipo de donante': 'Persona Moral Privada Extranjera'}, {'Especie ': '', 'Efectivo ': '94,554', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '15,733', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS'}, {'Monto': '18,552', 'Conceptos Ejercidos': 'VIGILANCIA Y SEGURIDAD'}, {'Monto': '296,282', 'Conceptos Ejercidos': 'HONORARIOS ASIMILADOS'}, {'Monto': '51,923', 'Conceptos Ejercidos': 'IVA ACREDITABLE DEDUCIBLE'}, {'Monto': '3,803', 'Conceptos Ejercidos': 'COMISIONES BANCARIAS'}, {'Monto': '6,712', 'Conceptos Ejercidos': 'EVENTOS Y GASTOS DE FIN DE AÑO'}, {'Monto': '1,266', 'Conceptos Ejercidos': 'SERVICIO FACTURA ELECTRONICA'}, {'Monto': '93,900', 'Conceptos Ejercidos': 'HONORARIOS A SOCIEDADES'}, {'Monto': '302', 'Conceptos Ejercidos': 'DISEÑO WEB'}, {'Monto': '28,126', 'Conceptos Ejercidos': 'DIVERSOS'}, {'Monto': '1,731', 'Conceptos Ejercidos': 'COMBUSTIBLES Y LUBRICANTES'}, {'Monto': '115,201', 'Conceptos Ejercidos': 'MANTENIMIENTO DE INSTALACIONES'}, {'Monto': '556', 'Conceptos Ejercidos': 'OTROS IMPUESTOS Y DERECHOS'}, {'Monto': '66,470', 'Conceptos Ejercidos': 'IMPRESION DE BOLETINES'}, {'Monto': '10,220', 'Conceptos Ejercidos': 'DEPRECIACIONES'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO  DE LA DOCUMENTACION SENSIBLE', 'Número de Beneficiarios': '728', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>{'Mision': 'APOYAR A MEJORAR LA CALIDAD DE VIDA DE LOS GRUPOS VULNERABLES DENTRO DE LA SOCIEDAD MEXICANA, SOBRE TODO DE AQUELLOS QUE VIVEN EN CONDICIOINES DE POBREZA Y DESIGUALDAD  POR CONDICIONES DE  EDAD, SEXO, ORIGEN O DISCAPACIDAD,  PROMOVIENDO Y CONTRIBUYENDO   AL DESARROLLO HUMANO, PERSONAL Y SOCIAL, A TRAVÉS DE LA EJECUCION  DE PROGRAMAS DE APOYO A LA SALUD, ALIMENTACIÓN, EDUCACION Y VIVIENDA.   PROMO', 'Vision': 'SER UNA ORGANIZACIÓN RECONOCIDA POR  EL APORTE CON NUESTRAS ACCIONES EN BENEFICIO DE QUIEN MÁS LO NECESITA A MEJORAR LA CONCIENCIA DE LA SOCIEDAD MEXICANA, ENFOCADOS  EN EL COMPROMISO Y EL RESPECTO A LA DIGNIDAD DE LAS PERSONAS Y LA HONESTIDAD.', 'Pagina web': 'https://anamalternativas@yahoo.com.mx', 'Anio de autorizacion': '2019', 'Socios o Asociados': 'HECTOR CANDIDO SANCHEZ GOMEZ,   LIDIA ROXANA SANCHEZ TAFOYA,  YAMILET SANCHEZ  TAFOYA', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '5', 'Monto total plantilla laboral': '2', 'Activo': '25,000', 'Pasivo': '0', 'Capital': '25,000', 'Gastos administracion': '6,000', 'Gastos operacion': '7,000', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': 'ENTREGA DE DESPENSAS', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'CUOTAS DE RECUPERACION', 'Monto': '15,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'VICEPRESIDENTE LIDIA ROXANA SANCHEZ TAFOYA', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'PRESIDENTE HECTOR CANDIDO SANCHEZ GOMEZ', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '15,000', 'Conceptos Ejercidos': 'PROGRAMA DE APOYOS ALIMENTICIOS'}]}, {'Donativos': [{'Donativos': '15,000', 'Beneficiarios': 'PERSONAS DE ESCASOS RECURSOS PERSONAS CON DISCAPACIDAD, Y ADULTOS MAYORES'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'ENTREA DE DESPENSAS A FAMILIAS DE ESCASOS RECURSOS', 'Número de Beneficiarios': '250', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'PROGRAMA DE SALUD MATERNO INFANTIL', 'Número de Beneficiarios': '70', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'ASISTENCIA SOCIAL PAQUETE DE SALUD E HIGIENE', 'Número de Beneficiarios': '150', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}]}]}</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creación y puesta en marcha de la red de orquestas sinfónicas y coros infantiles, juveniles y mixtos en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas públicas de educación básica y nivel medio superior.', 'Pagina web': 'http://www.esperanzaazteca.com/', 'Anio de autorizacion': '2019', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '20,614,528', 'Pasivo': '20,499,913', 'Capital': '114,615', 'Gastos administracion': '2,941,029', 'Gastos operacion': '66,764,995', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '15,747,742', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '41,892,743', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'INTERESES Y UTILIDAD CAMBIARIA', 'Monto': '449,105'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '23,290,767', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS CLASES PARA NIÑOS ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '244,819', 'Conceptos Ejercidos': 'FLETES TRANSPORTE DE INSTRUMENTOS'}, {'Monto': '42,368,979', 'Conceptos Ejercidos': 'COSTO ASISTENCIAL ORQUESTAS SINFÓNICAS ESPERANZA AZTECA'}, {'Monto': '494,978', 'Conceptos Ejercidos': 'RENTA DE SEDES PARA ORQUESTAS SINFONICAS ESPERANZA AZTECA'}]}, {'Donativos': [{'Donativos': '175,000', 'Beneficiarios': 'ESCUELA CRISTOBAL COLON AC'}, {'Donativos': '84,000', 'Beneficiarios': 'COLEGIO MONTFERRANT AC'}, {'Donativos': '106,452', 'Beneficiarios': 'FEDERACION MANO AMIGA AC'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jóvenes, frente a la crisis económica, la drogadicción, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '13,200', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jóvenes.', 'Número de Beneficiarios': '13,200', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Poner al alcance de niños y jóvenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, oportunidades, aprendizaje, comunicación con un lenguaje universal que es la música, entusiasmo personal, bienestar familiar, beneficios por la comunidad y amor por México.', 'Número de Beneficiarios': '13,200', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y zona Metropolitana', 'Vision': 'Ser Una Organizacion Reconocida a nivel nacional por el excelente trato y servicio antencion que se le brinda a los ancianos', 'Pagina web': 'http://asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Jaime Suarez Valencia, Pdte. Felisa Sanchez Fernandez, Srio. Esteban Garcia Reyes, Escrutadores Victor Alfonso Garcia Hernandez y Juana Rodriguez Contreras', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '10', 'Plantilla voluntariado': '13', 'Monto total plantilla laboral': '166,797', 'Activo': '13,155,681', 'Pasivo': '433,466', 'Capital': '12,561,210', 'Gastos administracion': '1,403', 'Gastos operacion': '908,913', 'Gastos representacion': '27,482', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '56,000', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '30,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '994,215', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': 'Medicamentos y Despensa por 56736', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '45,000', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'Ninguno', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'Ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '0', 'Conceptos Ejercidos': 'Ninguno'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'Ninguno'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Estancia asilo de ancianos', 'Número de Beneficiarios': '120', 'Entidad Federativa': 'Jalisco', 'Municipio': 'varios'}]}]}</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2010', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '12', 'Plantilla voluntariado': '', 'Monto total plantilla laboral': '350,592', 'Activo': '701,545,078', 'Pasivo': '42,185,459', 'Capital': '659,359,619', 'Gastos administracion': '0', 'Gastos operacion': '339,666,665', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '0', 'Efectivo ': '', 'Tipo de donante': 'Ninguno'}]}, {'OtrosIngresos': [{'Concepto': 'Ingresos por Venta y Edición de Libros', 'Monto': '339,020,000'}, {'Concepto': 'Ingresos por Intereses', 'Monto': '2,327'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'No aplica', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '200,226', 'Conceptos Ejercidos': 'Asesoría y Consultoría'}, {'Monto': '35,623', 'Conceptos Ejercidos': 'Otros Servicios'}, {'Monto': '4,987', 'Conceptos Ejercidos': 'Comisiones Bancarias'}, {'Monto': '339,000,000', 'Conceptos Ejercidos': 'Donativos'}, {'Monto': '51,237', 'Conceptos Ejercidos': 'Seguridad Social'}, {'Monto': '24,000', 'Conceptos Ejercidos': 'Depreciación'}, {'Monto': '350,592', 'Conceptos Ejercidos': 'Sueldos, Salarios y Gastos Relacionados'}]}, {'Donativos': [{'Donativos': '339,000,000', 'Beneficiarios': 'ICEL UNIVERSIDAD S.C.'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'No Aplica', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'No aplica'}]}]}</t>
+          <t>{'Mision': 'Darles un hogar digno en el que se encuentren felices y amados', 'Vision': 'Concluir la obra para poder trasladarlas, y poderles dar mejores espacios y areas verdes para que tengan mas comodidad, y acoger a muchos mas ya que la sociedad lo necesita, ya que el actual es muy pequeño ya que es una casa prestada', 'Pagina web': 'N/A', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA SANCHEZ FERNANDEZ, MARTIN HERNANDEZ, FRANCISCO LOPEZ AGUILAR, VICTOR ALFONSO GARCIA HERNANDEZ.', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '3', 'Plantilla voluntariado': '6', 'Monto total plantilla laboral': '30,000', 'Activo': '3,998,689', 'Pasivo': '0', 'Capital': '3,998,689', 'Gastos administracion': '2,999', 'Gastos operacion': '432,572', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': 'ARTICULOS DE LIMPIEZA', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MEDICAMENTOS Y ANALISIS CLINICOS', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MUEBLES Y ENSERES MENORES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'ARTICULOS DE LIMPIEZA', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MEDICAMENTOS Y ANALISIS CLINICOS', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MUEBLES Y ENSERES MENORES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'REEMBOLSO POR CAJA', 'Monto': '1,227'}, {'Concepto': 'RIFAS', 'Monto': '0'}, {'Concepto': 'CUOTAS DE RECUPERACION', 'Monto': '47,526'}, {'Concepto': 'BAZAR', 'Monto': '0'}, {'Concepto': 'INTERESES BANCARIOS', 'Monto': '236'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NO SE OTORGARON PERCEPCIONES', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '2,999', 'Conceptos Ejercidos': 'GASTOS FINANCIEROS'}, {'Monto': '5,478', 'Conceptos Ejercidos': 'OTROS'}, {'Monto': '2,159', 'Conceptos Ejercidos': 'SERVICIO TELEFONICO'}, {'Monto': '117,512', 'Conceptos Ejercidos': 'ACTIVOS FIJOS MOBILIARIO Y EQUIPO'}, {'Monto': '214', 'Conceptos Ejercidos': 'FLETES Y ACARREOS'}, {'Monto': '4,910', 'Conceptos Ejercidos': 'DIVERSOS'}, {'Monto': '0', 'Conceptos Ejercidos': 'PAPELERIA'}, {'Monto': '1,377', 'Conceptos Ejercidos': 'PAPELERIA Y UTILES'}, {'Monto': '2,467', 'Conceptos Ejercidos': 'ENERGIA ELECTRICA'}, {'Monto': '3,665', 'Conceptos Ejercidos': 'GAS'}, {'Monto': '138,489', 'Conceptos Ejercidos': 'MANTENIMIENTO E INSTALACION'}, {'Monto': '34,598', 'Conceptos Ejercidos': 'DESPENSA'}, {'Monto': '1,581,742', 'Conceptos Ejercidos': 'GASTOS POR OBRA CONSTRUCCION'}, {'Monto': '197,674', 'Conceptos Ejercidos': 'IVA ACREDITABLE'}, {'Monto': '2,731', 'Conceptos Ejercidos': 'MEDICAMENTO Y BOTIQUIN'}, {'Monto': '7,807', 'Conceptos Ejercidos': 'ALIMENTOS Y COMIDAS'}, {'Monto': '6,870', 'Conceptos Ejercidos': 'MANTENIMIENTO Y EQUIPO DE COMPUTO'}, {'Monto': '30,000', 'Conceptos Ejercidos': 'SUELDOS A ASIMILADOS'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NO SE OTORGARON'}]}], 'Actividades': [{'Actividades': []}]}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELÍAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TÉCNICOS Y DE PERSONAL ACADÉMICO', 'Vision': 'GARANTIZAR LA PROTECCIÓN, CONSERVACIÓN, RESTAURACIÓN Y RECUPERACIÓN, ASÍ COMO EL ESTUDIO, INVESTIGACIÓN, DIFUSIÓN DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRÁFICOS Y MUSEOGRÁFICOS QUE LO INTEGRAN.', 'Pagina web': 'www.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ALIAS CALLES ÁLVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMÍREZ ESPAÑA, LIC. MARÍA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '7', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '281,513', 'Activo': '751,085', 'Pasivo': '8,545', 'Capital': '742,540', 'Gastos administracion': '1,112,492', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '856', 'Tipo de donante': 'Persona Física Extranjera'}, {'Especie ': '', 'Efectivo ': '896', 'Tipo de donante': 'Persona Moral Privada Extranjera'}, {'Especie ': '', 'Efectivo ': '306,759', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '490,104', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,332', 'Conceptos Ejercidos': 'CORREOS Y ENVIOS'}, {'Monto': '271,711', 'Conceptos Ejercidos': 'VIGILANCIA Y SEGURIDAD'}, {'Monto': '8,140', 'Conceptos Ejercidos': 'RESTAURACIÓN DE LIBROS'}, {'Monto': '4,052', 'Conceptos Ejercidos': 'EVENTOS Y GASTOS DE FIN DE AÑO'}, {'Monto': '8,250', 'Conceptos Ejercidos': 'DISEÑO WEB'}, {'Monto': '56,271', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FÍSICAS'}, {'Monto': '281,513', 'Conceptos Ejercidos': 'ASIMILADOS A SALARIOS'}, {'Monto': '106,350', 'Conceptos Ejercidos': 'HONORARIOS A SOCIEDADES'}, {'Monto': '109,465', 'Conceptos Ejercidos': 'MANTENIMIENTO INSTALACIONES'}, {'Monto': '14,241', 'Conceptos Ejercidos': 'SIN REQUISITOS FISCALES'}, {'Monto': '40,688', 'Conceptos Ejercidos': 'MANTENIMIENTO ARCHIVO HISTÓRICO'}, {'Monto': '1,728', 'Conceptos Ejercidos': 'VIÁTICOS'}, {'Monto': '40,688', 'Conceptos Ejercidos': 'MANTENIMIENTO ARCHIVO HISTÓRICO'}, {'Monto': '1,728', 'Conceptos Ejercidos': 'VIÁTICOS'}, {'Monto': '40,688', 'Conceptos Ejercidos': 'MANTENIMIENTO ARCHIVO HISTÓRICO'}, {'Monto': '1,728', 'Conceptos Ejercidos': 'VIÁTICOS'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO DE LA DOCUMENTACIÓN SENSIBLE', 'Número de Beneficiarios': '562', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Impulsar los valores y el desarrollo integral de las familias a través del compromiso moral y económico. Además del desempeño físico-intelectual y emocional para lograr así una mejor calidad de vida.', 'Vision': 'Trabajar conjuntamente con el personal, alumnos, padres de familia, y demás miembros de la comunidad.', 'Pagina web': 'http://www.amigosdeaami.com', 'Anio de autorizacion': '2006', 'Socios o Asociados': 'Lourdes Legorreta Hernández, Beatriz Mariscal Asunsolo y Mónica Mariscal Asunsolo', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '686,520', 'Pasivo': '0', 'Capital': '686,520', 'Gastos administracion': '122,802', 'Gastos operacion': '632,678', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '15,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '3,433', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '19,130', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '25,000', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '2,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '17,150', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,492,386', 'Tipo de donante': 'Ninguno'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '18,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '28,258', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '15,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '12,680', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'RENDIMIENTO POR INVERSION', 'Monto': '18,354'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NA', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '354,552', 'Conceptos Ejercidos': 'EVENTOS'}, {'Monto': '145,221', 'Conceptos Ejercidos': 'HONORARIOS'}, {'Monto': '14,379', 'Conceptos Ejercidos': 'TELEFONOS'}]}, {'Donativos': [{'Donativos': '2,300,000', 'Beneficiarios': 'ASOCIACION MARIA INMACULADA A.C.'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Asistencia para el desarrollo integral de la comunidad de Palo Alto, Carretera México-Toluca', 'Número de Beneficiarios': '1', 'Entidad Federativa': 'Estado de México', 'Municipio': 'Palo Alto'}]}]}</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creacion y puesta en marcha de la red de 80 orquestas sinfonicas y coros infantiles, juveniles y mixtos  en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas publicas de educacion basica y nivel medio superior.', 'Pagina web': '', 'Anio de autorizacion': '2018', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '31,065,571', 'Pasivo': '27,634,521', 'Capital': '3,431,050', 'Gastos administracion': '6,420,925', 'Gastos operacion': '184,429,717', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '76,000,000', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '15,401,827', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '41,823,325', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'INTERESES Y UTILIDAD CAMBIARIA', 'Monto': '965,018'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '14,659,129', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS CLASES PARA NIÑOS ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '168,274,926', 'Conceptos Ejercidos': 'COSTO ASISTENCIAL ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '577,758', 'Conceptos Ejercidos': 'RENTA DE SEDES PARA ORQUESTAS SINFONICAS ESPERANZA AZTECA'}]}, {'Donativos': [{'Donativos': '275,000', 'Beneficiarios': 'ESCUELA CRISTOBAL COLON AC'}, {'Donativos': '220,000', 'Beneficiarios': 'FUNDACION COMUNITARIA PUEBLA IBP'}, {'Donativos': '90,000', 'Beneficiarios': 'COLEGIO MONTFERRANT AC'}, {'Donativos': '212,904', 'Beneficiarios': 'FEDERACION MANO AMIGA'}, {'Donativos': '120,000', 'Beneficiarios': 'FUNDACION BARCA AC'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jOvenes, frente a la crisis econOmica, la drogadicciOn, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Poner al alcance de niños y jovenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, Oportunidades, Aprendizaje, Comunicación con un lenguaje universal que es la música,entusiasmo personal, Bienestar familiar, Beneficios por la comunidad y Amor por México.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jOvenes.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y la zona metropolitana', 'Vision': 'Ser una organización reconocida a nivel nacional por el excelente trato y servicio atención que se le brinda a los ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Felisa sanchez fernandez juana rodriguez contreras esteban garcia reyes maria luisa Valderrama cervantes victor Alfonso garcia hernandez', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '6', 'Plantilla voluntariado': '20', 'Monto total plantilla laboral': '201,061', 'Activo': '12,801,693', 'Pasivo': '240,483', 'Capital': '12,561,210', 'Gastos administracion': '1,567', 'Gastos operacion': '1,214,948', 'Gastos representacion': '19,735', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '5,000', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '570,380', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '60431', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '80,763', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '160,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '60431', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'ninguno', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '0', 'Conceptos Ejercidos': 'ninguno'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'ningún particular recibo donativo'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'estancia asilo de ancianos', 'Número de Beneficiarios': '100', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Varios'}]}]}</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2010', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '531,928,612', 'Pasivo': '35,322,591', 'Capital': '496,606,021', 'Gastos administracion': '0', 'Gastos operacion': '307,947,139', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '0', 'Tipo de donante': 'No aplica'}]}, {'OtrosIngresos': [{'Concepto': 'Ingresos por Venta y Edición de Libros', 'Monto': '348,331,389'}, {'Concepto': 'Ingresos por Maquila', 'Monto': '6,346,162'}, {'Concepto': 'Ingresos por Intereses', 'Monto': '434,491'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'No aplica', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,173,748', 'Conceptos Ejercidos': 'Asesoria y Consultoria'}, {'Monto': '1,173,748', 'Conceptos Ejercidos': 'Asesoria y Consultoria'}]}, {'Donativos': [{'Donativos': '271,723,169', 'Beneficiarios': 'ICEL UNIVERSIDAD SC'}, {'Donativos': '25,000,000', 'Beneficiarios': 'UNIVERSIDAD DEL DESARROLLO PROFESIONAL SC'}, {'Donativos': '851,173', 'Beneficiarios': 'CRUZ ROJA MEXICANA'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'No aplica', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'No aplica'}]}]}</t>
+          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en condicion de abandono y maltrato de Guadalajara y la zona metropolitana brindando atencion integral al adulto mayor afreciendole un hogar digno con herramientas y personal necesario  para lograr un envejecimiento sano y activo', 'Vision': 'Ser una Organizacion reconocida a nivel nacional por excelente trato servicio y atencion que se le brinda a nuestros ancianos', 'Pagina web': 'http: asunciondemariaseniorshome.kerygs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA  SANCHEZ FERNANDEZ / VICTOR MANUEL IBARRA GUERRERO/ ESTEBAN GARCIA REYES/JOSE ANTONIO SEPULVEDA/VICTOR ALFONSO GARCIA HERNANDEZ', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '3', 'Plantilla voluntariado': '135', 'Monto total plantilla laboral': '225,011', 'Activo': '12,396,281', 'Pasivo': '3,055', 'Capital': '12,393,226', 'Gastos administracion': '549,600', 'Gastos operacion': '2,558,480', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'Cuotas de recuperacion', 'Monto': '177,600'}, {'Concepto': 'Colectas', 'Monto': '20,000'}, {'Concepto': 'Subsidios de Gobierno', 'Monto': '1,500,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': '.', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,500,000', 'Conceptos Ejercidos': 'Construccion de Instalaciones'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': '180'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Servicios Funerarios', 'Número de Beneficiarios': '4', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'estudios medicos especiales / terapias /analisis clinicos/homeopatia/ medicina alternativa', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Casa Hogar al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Servicio de Comedor al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'educacion basica', 'Número de Beneficiarios': '2', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Talleres', 'Número de Beneficiarios': '60', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'atencion integral al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Guadalajara'}]}]}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELIAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TECNICOS Y DE PERSONAL ACADEMICO.', 'Vision': 'GARANTIZAR LA PROTECCION, CONSERVACION, RESTAURACION Y RECUPERACION, ASI COMO EL ESTUDIO, INVESTIGACION, DIFUSION DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRAFICOS Y MUSEOGRAFICOS QUE LO INTEGRAN.', 'Pagina web': 'www.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ALIAS CALLES ALVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMIREZ ESPAÑA, LIC. MARIA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '1,056,567', 'Pasivo': '150', 'Capital': '1,056,417', 'Gastos administracion': '734,106', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '257,490', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '537,295', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '31,667', 'Tipo de donante': 'Persona Física Extranjera'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO DE LA DOCUMENTACION SENCIBLE', 'Número de Beneficiarios': '489', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Impulsar los valores y el desarrollo integral de las familias a través del compromiso moral y económico. Además del desempeño físico-intelectual y emocional para lograr así una mejor calidad de vida.', 'Vision': 'Trabajar conjuntamente con el personal, alumnos, padres de familia, y demás miembros de la comunidad.', 'Pagina web': 'http://www.amigosdeaami.com', 'Anio de autorizacion': '2006', 'Socios o Asociados': 'Lourdes Legorreta Hernández, Beatriz Mariscal Asunsolo y Mónica Mariscal Asunsolo', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '1,057,610', 'Pasivo': '0', 'Capital': '1,057,610', 'Gastos administracion': '135,006', 'Gastos operacion': '672,074', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'RENDIMIENTO POR INVERSION', 'Monto': '14,683'}, {'Concepto': 'OTROS', 'Monto': '19,488'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'N/A', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '500,634', 'Conceptos Ejercidos': 'EVENTOS'}, {'Monto': '14,379', 'Conceptos Ejercidos': 'TELEFONOS'}, {'Monto': '120,628', 'Conceptos Ejercidos': 'HONORARIOS'}]}, {'Donativos': [{'Donativos': '1,650,000', 'Beneficiarios': 'ASOCIACIÓN MARÍA INMACULADA A.C.'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Asistencia para el desarrollo integral de la comunidad de Palo Alto, Carretera México-Toluca', 'Número de Beneficiarios': '1', 'Entidad Federativa': 'Estado de México', 'Municipio': 'Palo Alto'}]}]}</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creacion y puesta en marcha de la red de 80 orquestas sinfonicas y coros infantiles, juveniles y mixtos  en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas publicas de educacion basica y nivel medio superior.', 'Pagina web': 'http://www.esperanzaazteca.com/', 'Anio de autorizacion': '2017', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '74,866,248', 'Pasivo': '14,774,726', 'Capital': '60,091,522', 'Gastos administracion': '7,411,920', 'Gastos operacion': '201,978,098', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '152,004,796', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '55,151,949', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '11,856,037', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': 'INSTRUMENTOS MUSICALES', 'Efectivo ': '', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'INTERESES Y UTILIDAD CAMBIARIA', 'Monto': '1,428,468'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '185,042,684', 'Conceptos Ejercidos': 'COSTO ASISTENCIAL ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '681,745', 'Conceptos Ejercidos': 'RENTA DE SEDES PARA ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '15,473,840', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS CLASES PARA NIÑOS ORQUESTAS SINFONICAS ESPERANZA AZTECA'}]}, {'Donativos': [{'Donativos': '125,000', 'Beneficiarios': 'CONSERVATORIO DE LAS ROSAS AC'}, {'Donativos': '179,829', 'Beneficiarios': 'COLEGIO MONTFERRANT AC'}, {'Donativos': '325,000', 'Beneficiarios': 'CENTRO EDUCATIVO CUALCAN ACAPULCO SC'}, {'Donativos': '30,000', 'Beneficiarios': 'FUNDACION BARCA AC'}, {'Donativos': '120,000', 'Beneficiarios': 'ESCUELA CRISTOBAL COLON AC'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jóvenes.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jóvenes, frente a la crisis económica, la drogadicción, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Poner al alcance de niños y jovenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, Oportunidades, Aprendizaje, Comunicación con un lenguaje universal que es la música,entusiasmo personal, Bienestar familiar, Beneficios por la comunidad y Amor por México.', 'Número de Beneficiarios': '17,000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y la zona metropolitana', 'Vision': 'Ser una organización reconocida a nivel nacional por el excelente trato y servicio y atención que se le brinda a los ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Felisa Sánchez Fernández  Alonso García Hernández esteban garcia Antonio sepulveda', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '8', 'Plantilla voluntariado': '25', 'Monto total plantilla laboral': '201,343', 'Activo': '13,163,696', 'Pasivo': '164,894', 'Capital': '12,998,802', 'Gastos administracion': '8,497', 'Gastos operacion': '880,868', 'Gastos representacion': '27,322', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'cuotas de recuperacion', 'Monto': '748,750'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '998,814', 'Conceptos Ejercidos': 'asilo de ancianos medicamentos alimentación estancia defuncion'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'ninguno'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'estancia asilo de ancianos', 'Número de Beneficiarios': '90', 'Entidad Federativa': 'Jalisco', 'Municipio': 'varios'}]}]}</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2010', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '275,751,357', 'Pasivo': '22,254,307', 'Capital': '253,497,050', 'Gastos administracion': '0', 'Gastos operacion': '208,637,083', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '0', 'Tipo de donante': 'No aplica'}]}, {'OtrosIngresos': [{'Concepto': 'Ingresos por Venta y Edición de Libros.', 'Monto': '423,131,052'}, {'Concepto': 'Ingresos por Intereses.', 'Monto': '37,465'}, {'Concepto': 'Ingresos por Maquila.', 'Monto': '6,085,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'No aplica.', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '15,000,000', 'Beneficiarios': 'LAMAR MEXICANA A.C.'}, {'Donativos': '172,533,656', 'Beneficiarios': 'ICEL UNIVERSIDAD S.C.'}, {'Donativos': '15,000,000', 'Beneficiarios': 'INSTITUTO EL DISEÑADOR DE LA MODA S.C.'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'No aplica.', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'No aplica.'}]}]}</t>
+          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en condicion de abandono y maltrato de Guadalajara y la zona Metropolitana brindando atencion', 'Vision': 'ser una organizacion reconocida a nivel nacional por el excelente trato servicio y atencion que se les brinda a nuestros ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA SANCHEZ FERNANDEZ PRESIDENTE DEL CONSEJO VICTOR ALFONSO GARCIA HERNANDEZ SECRETARIO ESTEBAN GARCIA REYES TESORERO JUANA RODRIGUEZ CONTRERAS VOCAL  MARIA LUISA VALDERRAMA CERVANTES VOCAL', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '13', 'Plantilla voluntariado': '11', 'Monto total plantilla laboral': '466,797', 'Activo': '13,130,203', 'Pasivo': '222,889', 'Capital': '12,907,314', 'Gastos administracion': '19,996', 'Gastos operacion': '970,599', 'Gastos representacion': '50,802', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'cuotas de recuperacion', 'Monto': '1,019,776'}, {'Concepto': 'subsidios de gobierno', 'Monto': '399,994'}, {'Concepto': 'colectas', 'Monto': '41,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguna', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,929,952', 'Conceptos Ejercidos': 'asilo de ancianos'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'Mercedes Sanchez Maria de laLuz Ramos Larios Luisa Macias Martinez Juan Jose Rito Villafan Vicente Guzman Galvan Antonio Castillo Castillo Patricia Araceli Coronado Hernandez Leoncio Gomez Jose Manuel Peredia Garcia Lorenzo Bautista Ramirez Maria Guadalupe Carrillo Soto Sara Rojas Trujillo Ramon Quintana Jose Miguel de Jesus Gonzalez Islas Marcelino Arellano Valin Vicente Ruiz Canel'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'atencion integral al adulto mayor', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': '34'}, {'Actividad': 'servicio de comedor al adulto mayor', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}, {'Actividad': 'estudios medicos especiales terapias analisis clinicos', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}, {'Actividad': 'talleres', 'Número de Beneficiarios': '60', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}]}]}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELIAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TECNICOS Y DE PERSONAL ACADEMICO.', 'Vision': 'GARANTIZAR LA PROTECCION, CONSERVACION, RESTAURACION Y RECUPERACION, ASI COMO EL ESTUDIO, INVESTIGACION, DIFUSION DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRAFICOS Y MUSEOGRAFICOS QUE LO INTEGRAN.', 'Pagina web': 'www.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ALIAS CALLES ALVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMIREZ ESPAÑA, LIC. MARIA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '964,222', 'Pasivo': '150', 'Capital': '964,072', 'Gastos administracion': '701,844', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '8,455', 'Tipo de donante': 'Persona Física Extranjera'}, {'Especie ': '', 'Efectivo ': '583,848', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '371,488', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO DE LA DOCUMENTACION SENSIBLE', 'Número de Beneficiarios': '445', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Impulsar los valores y el desarrollo integral de las familias a través del compromiso moral y económico. Además del desempeño físico-intelectual y emocional para lograr así una mejor calidad de vida.', 'Vision': 'Trabajar conjuntamente con el personal, alumnos, padres de familia, y demás miembros de la comunidad.', 'Pagina web': 'http://www.amigosdeaami.com', 'Anio de autorizacion': '2006', 'Socios o Asociados': 'Lourdes Legorreta Hernández, Beatriz Mariscal Asunsolo y Mónica Mariscal Asunsolo', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '736,903', 'Pasivo': '0', 'Capital': '736,903', 'Gastos administracion': '167,550', 'Gastos operacion': '726,687', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '15,695', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '20,888', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '15,695', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '20,888', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '15,695', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '20,888', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'Otros', 'Monto': '20,250'}, {'Concepto': 'Rendimiento por inversion', 'Monto': '7,576'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'N/A', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '443,710', 'Conceptos Ejercidos': 'Eventos'}, {'Monto': '110,590', 'Conceptos Ejercidos': 'Honorarios'}, {'Monto': '24,000', 'Conceptos Ejercidos': 'Energía Eléctrica'}]}, {'Donativos': [{'Donativos': '4,400,000', 'Beneficiarios': 'Asociación María Inmaculada A.C.'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Asistencia para el desarrollo integral de la comunidad de Palo Alto, Carretera México-Toluca', 'Número de Beneficiarios': '1', 'Entidad Federativa': 'Estado de México', 'Municipio': 'Palo Alto'}]}]}</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creacion y puesta en marcha de la red de 80 orquestas sinfonicas y coros infantiles, juveniles y mixtos  en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas publicas de educacion basica y nivel medio superior.', 'Pagina web': 'http://www.esperanzaazteca.com/', 'Anio de autorizacion': '2016', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '58,735,076', 'Pasivo': '10,787,390', 'Capital': '47,947,686', 'Gastos administracion': '8,285,475', 'Gastos operacion': '224,078,798', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '37,245,772', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': 'INSTRUMENTOS MUSICALES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '182,111,480', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '5,058,715', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'INTERESES BANCARIOS', 'Monto': '287,851'}, {'Concepto': 'UTILIDAD CAMBIARIA', 'Monto': '15,011'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '418,088', 'Conceptos Ejercidos': 'RENTA DE SEDES PARA ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '552,305', 'Conceptos Ejercidos': 'GASTOS FINANCIEROS'}, {'Monto': '212,785,267', 'Conceptos Ejercidos': 'COSTO ASISTENCIAL ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '10,323,138', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS'}]}, {'Donativos': [{'Donativos': '2,077,672', 'Beneficiarios': 'FUNDACION COMUNITARIA PUEBLA IBP'}, {'Donativos': '461,352', 'Beneficiarios': 'NIÑOS PARA UN MUNDO MEJOR AC'}, {'Donativos': '72,000', 'Beneficiarios': 'COLEGIO MONTFERRANT AC'}, {'Donativos': '80,000', 'Beneficiarios': 'FUNDACION BARCA AC'}, {'Donativos': '375,000', 'Beneficiarios': 'INSTITUTO INTERNACIONAL DE DERECHO CULTURAL Y DESARRLLO SUSTENTABLE IIDECUL DESUS AC'}, {'Donativos': '300,000', 'Beneficiarios': 'ESCUELA CRISTOBAL COLON AC'}, {'Donativos': '140,000', 'Beneficiarios': 'PODER CIVICO AC'}, {'Donativos': '177,429', 'Beneficiarios': 'CENTRO EDUCATIVO CUALCAN ACAPULCO SC'}, {'Donativos': '181,500', 'Beneficiarios': 'ACADEMIA DE MUSICA DEL PALACIO DE MINERIA AC'}, {'Donativos': '150,000', 'Beneficiarios': 'CONSERVATORIO DE LAS ROSAS AC'}, {'Donativos': '20,000', 'Beneficiarios': 'INSTITUTO DE FOMENTO E INVESTIGACION EDUCATIVA AC'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Poner al alcance de niños y jovenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, Oportunidades, Aprendizaje, Comunicación con un lenguaje universal que es la música,entusiasmo personal, Bienestar familiar, Beneficios por la comunidad y Amor por México.', 'Número de Beneficiarios': '17000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jóvenes.', 'Número de Beneficiarios': '17000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jóvenes, frente a la crisis económica, la drogadicción, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '17000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en condicion de abandono y maltrato de Guadalajara y la zona Metropolitana brindando atencion', 'Vision': 'ser una organizacion reconocida a nivel nacional por el excelente trato servicio y atencion que se les brinda a nuestros ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA SANCHEZ FERNANDEZ PRESIDENTE DEL CONSEJO VICTOR ALFONSO GARCIA HERNANDEZ SECRETARIO ESTEBAN GARCIA REYES TESORERO JUANA RODRIGUEZ CONTRERAS VOCAL  MARIA LUISA VALDERRAMA CERVANTES VOCAL', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '13', 'Plantilla voluntariado': '11', 'Monto total plantilla laboral': '466,797', 'Activo': '13,130,203', 'Pasivo': '222,889', 'Capital': '12,907,314', 'Gastos administracion': '19,996', 'Gastos operacion': '970,599', 'Gastos representacion': '50,802', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'colectas', 'Monto': '41,000'}, {'Concepto': 'subsidios de gobierno', 'Monto': '399,994'}, {'Concepto': 'cuotas de recuperacion', 'Monto': '1,019,776'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguna', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,929,952', 'Conceptos Ejercidos': 'asilo de ancianos'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'Mercedes Sanchez Maria de laLuz Ramos Larios Luisa Macias Martinez Juan Jose Rito Villafan Vicente Guzman Galvan Antonio Castillo Castillo Patricia Araceli Coronado Hernandez Leoncio Gomez Jose Manuel Peredia Garcia Lorenzo Bautista Ramirez Maria Guadalupe Carrillo Soto Sara Rojas Trujillo Ramon Quintana Jose Miguel de Jesus Gonzalez Islas Marcelino Arellano Valin Vicente Ruiz Canel'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'talleres', 'Número de Beneficiarios': '60', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}, {'Actividad': 'atencion integral al adulto mayor', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': '34'}, {'Actividad': 'estudios medicos especiales terapias analisis clinicos', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}, {'Actividad': 'servicio de comedor al adulto mayor', 'Número de Beneficiarios': '79', 'Entidad Federativa': 'Jalisco', 'Municipio': 'tlaquepaque'}]}]}</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2010', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '', 'Plantilla voluntariado': '', 'Monto total plantilla laboral': '0', 'Activo': '11,832', 'Pasivo': '0', 'Capital': '11,832', 'Gastos administracion': '0', 'Gastos operacion': '6,728', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '0', 'Tipo de donante': 'No aplica'}]}, {'OtrosIngresos': [{'Concepto': 'No Aplica', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'No Aplica', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'No Aplica'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'No Aplica', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'No Aplica'}]}]}</t>
+          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y la zona metropolitana', 'Vision': 'Ser una organización reconocida a nivel nacional por el excelente trato y servicio y atención que se le brinda a los ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Felisa Sánchez Fernández  Alonso García Hernández esteban garcia Antonio sepulveda', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '8', 'Plantilla voluntariado': '25', 'Monto total plantilla laboral': '201,343', 'Activo': '13,163,696', 'Pasivo': '164,894', 'Capital': '12,998,802', 'Gastos administracion': '8,497', 'Gastos operacion': '880,868', 'Gastos representacion': '27,322', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'cuotas de recuperacion', 'Monto': '748,750'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '998,814', 'Conceptos Ejercidos': 'asilo de ancianos medicamentos alimentación estancia defuncion'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'ninguno'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'estancia asilo de ancianos', 'Número de Beneficiarios': '90', 'Entidad Federativa': 'Jalisco', 'Municipio': 'varios'}]}]}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELIAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TECNICOS Y DE PERSONAL ACADEMICO.', 'Vision': 'GARANTIZAR LA PROTECCION, CONSERVACION, RESTAURACION Y RECUPERACION, ASI COMO EL ESTUDIO, INVESTIGACION, DIFUSION DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRAFICOS Y MUSEOGRAFICOS QUE LO INTEGRAN.', 'Pagina web': 'WWW.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ALIAS CALLES ALVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMIREZ ESPAÑA, LIC. MARIA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '702,123', 'Pasivo': '150', 'Capital': '701,973', 'Gastos administracion': '645,664', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '44,780', 'Tipo de donante': 'Persona Física Extranjera'}, {'Especie ': '', 'Efectivo ': '736', 'Tipo de donante': 'Persona Moral Privada Extranjera'}, {'Especie ': '', 'Efectivo ': '136,630', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '471,239', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO  DE LA DOCUMENTACION SENSIBLE', 'Número de Beneficiarios': '619', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Impulsar los valores y el desarrollo integral de las familias a través del compromiso moral y económico. Además del desempeño físico-intelectual y emocional para lograr así una mejor calidad de vida', 'Vision': 'Trabajar conjuntamente con el personal, alumnos, padres de familia, y demás miembros de la comunidad', 'Pagina web': 'http://www.amigosdeaami.com', 'Anio de autorizacion': '2006', 'Socios o Asociados': 'Lourdes Legorreta Hernández, Beatriz Mariscal Asunsolo y Mónica Mariscal Asunsolo', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '', 'Monto total plantilla laboral': '0', 'Activo': '2,405,921', 'Pasivo': '1,471', 'Capital': '2,404,450', 'Gastos administracion': '120,829', 'Gastos operacion': '643,855', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'Otros', 'Monto': '5,110'}, {'Concepto': 'Rendimiento por inversion', 'Monto': '4,228'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'N/A', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '422,223', 'Conceptos Ejercidos': 'Eventos'}, {'Monto': '30,875', 'Conceptos Ejercidos': 'Energía Eléctrica'}, {'Monto': '13,317', 'Conceptos Ejercidos': 'Teléfono'}, {'Monto': '100,699', 'Conceptos Ejercidos': 'Honorarios'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'NINGUNO', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Distrito Federal', 'Municipio': 'N/A'}]}]}</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{'Mision': 'EN LA ASOCIACION TENEMOS LA MISION DE INCLUIR A LOS GRUPOS VULNERABLES A NUESTROS PROGRAMAS', 'Vision': 'INCLUIR A TODOS LOS GRUPOS VULNERABLES A LOS BENEFICIOS QUE LOGREMOS AL GESTIONAR ANTE INSTANCIAS GUBERNAMENTALES Y PRIVADAS APOYOS PARA MEJORAR SU NIVEL DE VIDA', 'Pagina web': '', 'Anio de autorizacion': '2015', 'Socios o Asociados': 'HECTOR CANDIDO SANCHEZ GOMEZ, NANCY BLANCA ESTELA MENDOZA TAFOYA, LIDIA TAFOYA PADILLA, LIDIA ROXANA SANCHEZ TAFOYA,FRANCISCO CORTES SANTIAGO', 'Rubros autorizados': ['L. Organizaciones Civiles y Fideicomisos de Desarrollo Social.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '0', 'Pasivo': '0', 'Capital': '0', 'Gastos administracion': '0', 'Gastos operacion': '1,500', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': 'TELMEZ JUGUETES 150 PERSONAS', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'CUOTAS DE RECUPERACION', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'VICEPRESIDENTE C. LIDIA TAFOYA PADILLA', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'PRESIDENTE C. HECTOR CANDIDO SANCHEZ GOMEZ', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'VOCAL C. FRANCISCO CORTES SANTIAGO', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'TESORERO C. LIDIA ROXANA SANCHEZ TAFOYA', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'PRESIDENTE C. HECTOR CANDIDO SANCHEZ GOMEZ', 'Total de percepciones netas': '0'}, {'Cargo ó Nombramiento': 'SECRETARIO C. NANCY BLANCA ESTELA TAFOYA MENDOZA', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,500', 'Conceptos Ejercidos': 'GASTOS DE OPERACION'}]}, {'Donativos': [{'Donativos': '1,000', 'Beneficiarios': 'PAÑALES PARA ADULTO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'POPULAR ENTREGA DE JUGUETAS', 'Número de Beneficiarios': '150', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}]}]}</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creacion y puesta en marcha de la red de 80 orquestas sinfonicas y coros infantiles, juveniles y mixtos  en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas publicas de educacion basica y nivel medio superior.', 'Pagina web': 'http://www.esperanzaazteca.com/', 'Anio de autorizacion': '2015', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '66,937,974', 'Pasivo': '7,328,108', 'Capital': '59,609,866', 'Gastos administracion': '7,981,953', 'Gastos operacion': '222,198,548', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '27,672,432', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '196,217,200', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'INSTRUMENTOS MUSICALES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,279,503', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'UTILIDAD CAMBIARIA', 'Monto': '34,615'}, {'Concepto': 'INTERESES BANCARIOS', 'Monto': '495,338'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '8,977,348', 'Conceptos Ejercidos': 'HONORARIOS PERSONAS FISICAS'}, {'Monto': '206,001,009', 'Conceptos Ejercidos': 'COSTO ASISTENCIAL ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '582,108', 'Conceptos Ejercidos': 'IMPUESTO SOBRE LA RENTA'}, {'Monto': '6,286,031', 'Conceptos Ejercidos': 'GASTOS POR IVA'}, {'Monto': '352,052', 'Conceptos Ejercidos': 'GASTOS FINANCIEROS'}]}, {'Donativos': []}], 'Actividades': [{'Actividades': [{'Actividad': 'Poner al alcance de niños y jovenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, Oportunidades, Aprendizaje, Comunicación con un lenguaje universal que es la música,entusiasmo personal, Bienestar familiar, Beneficios por la comunidad y Amor por México.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jóvenes.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jóvenes, frente a la crisis económica, la drogadicción, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en condicion de abandono y maltrato de Guadalajara y la zona metropolitana brindando atencion integral al adulto mayor afreciendole un hogar digno con herramientas y personal necesario  para lograr un envejecimiento sano y activo', 'Vision': 'Ser una Organizacion reconocida a nivel nacional por excelente trato servicio y atencion que se le brinda a nuestros ancianos', 'Pagina web': 'http: asunciondemariaseniorshome.kerygs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA  SANCHEZ FERNANDEZ / VICTOR MANUEL IBARRA GUERRERO/ ESTEBAN GARCIA REYES/JOSE ANTONIO SEPULVEDA/VICTOR ALFONSO GARCIA HERNANDEZ', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '3', 'Plantilla voluntariado': '135', 'Monto total plantilla laboral': '225,011', 'Activo': '12,396,281', 'Pasivo': '3,055', 'Capital': '12,393,226', 'Gastos administracion': '549,600', 'Gastos operacion': '2,558,480', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': []}, {'OtrosIngresos': [{'Concepto': 'Cuotas de recuperacion', 'Monto': '177,600'}, {'Concepto': 'Subsidios de Gobierno', 'Monto': '1,500,000'}, {'Concepto': 'Colectas', 'Monto': '20,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': '.', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '1,500,000', 'Conceptos Ejercidos': 'Construccion de Instalaciones'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': '180'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'educacion basica', 'Número de Beneficiarios': '2', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Talleres', 'Número de Beneficiarios': '60', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Servicio de Comedor al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'atencion integral al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Guadalajara'}, {'Actividad': 'Casa Hogar al adulto mayor', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'estudios medicos especiales / terapias /analisis clinicos/homeopatia/ medicina alternativa', 'Número de Beneficiarios': '180', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}, {'Actividad': 'Servicios Funerarios', 'Número de Beneficiarios': '4', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Tlaquepaque'}]}]}</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2010', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '', 'Plantilla voluntariado': '', 'Monto total plantilla laboral': '0', 'Activo': '4,561', 'Pasivo': '45,000', 'Capital': '-40,439', 'Gastos administracion': '0', 'Gastos operacion': '18,903', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '0', 'Tipo de donante': 'No aplica'}]}, {'OtrosIngresos': [{'Concepto': 'No aplica', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'No aplica', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'No aplica'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'No aplica', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'No aplica'}]}]}</t>
+          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y la zona metropolitana', 'Vision': 'Ser una organización reconocida a nivel nacional por el excelente trato y servicio atención que se le brinda a los ancianos', 'Pagina web': 'http:asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Felisa sanchez fernandez juana rodriguez contreras esteban garcia reyes maria luisa Valderrama cervantes victor Alfonso garcia hernandez', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '6', 'Plantilla voluntariado': '20', 'Monto total plantilla laboral': '201,061', 'Activo': '12,801,693', 'Pasivo': '240,483', 'Capital': '12,561,210', 'Gastos administracion': '1,567', 'Gastos operacion': '1,214,948', 'Gastos representacion': '19,735', 'Ingresos': [{'Ingresos': [{'Especie ': '60431', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '80,763', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '570,380', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '60431', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '160,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '5,000', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'ninguno', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '0', 'Conceptos Ejercidos': 'ninguno'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'ningún particular recibo donativo'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'estancia asilo de ancianos', 'Número de Beneficiarios': '100', 'Entidad Federativa': 'Jalisco', 'Municipio': 'Varios'}]}]}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'Mision': 'COADYUVAR LOS ARCHIVOS PLUTARCO ELIAS CALLES Y FERNANDO TORREBLANCA EN LO QUE SE REFIERE AL APOYO DE SERVICIOS TECNICOS Y DE PERSONAL ACADEMICO.', 'Vision': 'GARANTIZAR LA PROTECCION, CONSERVACION, RESTAURACION Y RECUPERACION, ASI COMO EL ESTUDIO, INVESTIGACION, DIFUSION DE LOS MATERIALES DOCUMENTALES, HEMEROGRAFICOS, FOTOGRAFICOS Y MUSEOGRAFICOS QUE LO INTEGRAN.', 'Pagina web': 'www.fapecft.org.mx', 'Anio de autorizacion': '2004', 'Socios o Asociados': 'LIC. NORMA MERELES TORREBLANCA DE OGARRIO, LIC. FERNANDO ELIAS CALLES ALVAREZ, LIC. RAFAEL FERNANDO ROMERO TORREBLANCA, LIC. RODOLFO OGARRIO RAMIREZ ESPAÑA, LIC. MARIA DEL CARMEN AGUILAR ZINSER.', 'Rubros autorizados': ['C. Organizaciones Civiles y Fideicomisos para la Investigación Científica o Tecnológica.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '694,252', 'Pasivo': '0', 'Capital': '694,252', 'Gastos administracion': '718,309', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '558', 'Tipo de donante': 'Persona Moral Privada Extranjera'}, {'Especie ': '', 'Efectivo ': '672,302', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '5,824', 'Tipo de donante': 'Persona Física Extranjera'}, {'Especie ': '0', 'Efectivo ': '', 'Tipo de donante': 'Ninguno'}, {'Especie ': '', 'Efectivo ': '106,464', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'NINGUNO', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NINGUNO', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NINGUNO'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'RESGUARDO DE LA DOCUMENTACION SENSIBLE', 'Número de Beneficiarios': '589', 'Entidad Federativa': 'Nacional', 'Municipio': 'VARIOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Impulsar los valores y el desarrollo integral de las familias a través del compromiso moral y económico. Además del desempeño físico intelectual y emocional para lograr así una mejor calidad de vida.', 'Vision': 'Trabajar conjuntamente con el personal, alumnos, padres de familia, y demás miembros de la comunidad.', 'Pagina web': 'www.amigosdeaami.com', 'Anio de autorizacion': '2006', 'Socios o Asociados': 'Lourdes Legorreta Hernández, Beatriz Mariscal Asunsolo y Mónica Mariscal Asunsolo', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '775,740', 'Pasivo': '39,456', 'Capital': '736,284', 'Gastos administracion': '149,848', 'Gastos operacion': '3,072,082', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '11,875', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '17,500', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '2,500', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '17,500', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '17,500', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '2,684,341', 'Tipo de donante': 'Ninguno'}, {'Especie ': '', 'Efectivo ': '60,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '17,500', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '17,500', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '2,500', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '20,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,684,341', 'Tipo de donante': 'Ninguno'}, {'Especie ': '', 'Efectivo ': '20,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,400', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '27,500', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '27,500', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '20,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '60,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '62,225', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '30,000', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '4,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,400', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,400', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '2,400', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'Otros', 'Monto': '2,000'}, {'Concepto': 'Rendimiento por Inversión', 'Monto': '6,043'}, {'Concepto': 'Rendimiento por Inversión', 'Monto': '6,043'}, {'Concepto': 'Otros', 'Monto': '2,000'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'N/A', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '129,571', 'Conceptos Ejercidos': 'Honorarios'}, {'Monto': '17,906', 'Conceptos Ejercidos': 'Teléfono'}, {'Monto': '210,814', 'Conceptos Ejercidos': 'Eventos'}, {'Monto': '210,814', 'Conceptos Ejercidos': 'Eventos'}, {'Monto': '31,440', 'Conceptos Ejercidos': 'Papeleria'}, {'Monto': '17,906', 'Conceptos Ejercidos': 'Teléfono'}, {'Monto': '129,571', 'Conceptos Ejercidos': 'Honorarios'}, {'Monto': '31,440', 'Conceptos Ejercidos': 'Papeleria'}]}, {'Donativos': [{'Donativos': '2,750,000', 'Beneficiarios': 'Asociación Amigos de Maria Inmaculada IAP'}, {'Donativos': '2,750,000', 'Beneficiarios': 'Asociación Amigos de Maria Inmaculada IAP'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Asistencia para el desarrollo integral de la comunidad de Palo Alto, Carretera México-Toluca', 'Número de Beneficiarios': '1', 'Entidad Federativa': 'Estado de México', 'Municipio': 'Palo Alto'}, {'Actividad': 'Asistencia para el desarrollo integral de la comunidad de Palo Alto, Carretera México-Toluca', 'Número de Beneficiarios': '1', 'Entidad Federativa': 'Estado de México', 'Municipio': 'Palo Alto'}]}]}</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>{'Mision': 'SER UNA ORGANIZACION RECONOCIDA POR NUESTRA CONSTANTE ACTIVIDAD EN BENEFICIO DE QUIEN MAS LOS NECESITE DEMOSTRANDOLO CON ACCIONES REALES DE FORMA COMPROMETIDA HONESTA Y FILANTROPICA', 'Vision': 'MEJORAR LA CALIDAD DE VIDA DE LOS GRUPOS VULNERABLES SOBRE TODO DE AQUELLOS QUE VIVEN EN POBREZA EXTREMA COADYUVANDO EN SALUD, ALIMENTACION, PREVENCION Y CAPACITACION ASIMISMO COMO MEJORAR LA CONIDICION DE LA POBLACION EN SITUACION DE VIOLENCIA COMPROMETIDOS A LA ATENCION ORIENTACION CAPACITACION Y CANALIZACION EN CONSONANCIA MEDIANTE EVENTOS PREVENTIVOS, LUDICOS, CULTURALES, DEPORTIVOS Y EFLUVIO', 'Pagina web': '', 'Anio de autorizacion': '2014', 'Socios o Asociados': 'HECTOR CANDIDO SANCHEZ GOMEZ, LIDIA TAFOYA PADILLA, NANCY BLANCA ESTELA MENDOZA TAFOYA, LIDIA ROXANA SANCHEZ TAFOYA, FRANCISCO CORTEZ SANTIAGO.', 'Rubros autorizados': ['No aplica'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '0', 'Pasivo': '0', 'Capital': '0', 'Gastos administracion': '0', 'Gastos operacion': '0', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': 'DONATIVO EN ESPECIE', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'CUOTAS', 'Monto': '4,000'}]}], 'Egresos': [{'Egresos': []}, {'MontosConceptos': [{'Monto': '4,000', 'Conceptos Ejercidos': 'DESPENSAS'}]}, {'Donativos': [{'Donativos': '4,000', 'Beneficiarios': 'PERSONAS DE LA TERCERA EDAD, NIÑEZ, PERSONAS CON DISCAPACIDAD Y MADRES SOLTERAS'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'LUDOTECAS INFANTILES', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Distrito Federal', 'Municipio': 'IZTAPALAPA'}, {'Actividad': 'TALLERES PREVENTIVOS', 'Número de Beneficiarios': '1000', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'LUDOTECAS INFANTILES', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'EVENTOS DEPORTIVOS', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'EVENTOS ADULTOS MAYORES', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'EVENTOS CULTURALES', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Distrito Federal', 'Municipio': 'IZTAPALAPA'}, {'Actividad': 'EVENTOS CULTURALES', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}, {'Actividad': 'EVENTOS DEPORTIVOS', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Distrito Federal', 'Municipio': 'IZTAPALAPA'}, {'Actividad': 'ENTREGA DE ABASTO POPULAR', 'Número de Beneficiarios': '500', 'Entidad Federativa': 'Estado de México', 'Municipio': 'NEZAHUALCOYOTL'}]}]}</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Promover, fomentar, estimular y difundir las bellas artes, la música, la danza y la arquitectura. Brindar a niños y adolescentes de escasos recursos en todo el país, la oportunidad de desarrollar los más altos valores humanos: trabajo en equipo, orientación al logro y la excelencia, esfuerzo y disciplina a través de la enseñanza y la práctica de la música sinfónica y coral.', 'Vision': 'Creacion y puesta en marcha de la red de 80 orquestas sinfonicas y coros infantiles, juveniles y mixtos  en el territorio mexicano, que impacten directamente a poblaciones infantiles marginadas pertenecientes preferentemente a las escuelas publicas de educacion basica y nivel medio superior.', 'Pagina web': 'http://www.esperanzaazteca.com/', 'Anio de autorizacion': '2014', 'Socios o Asociados': '', 'Rubros autorizados': ['D. Organizaciones Civiles y Fideicomisos Culturales.'], 'Plantilla laboral': '0', 'Plantilla voluntariado': '0', 'Monto total plantilla laboral': '0', 'Activo': '81,473,813', 'Pasivo': '12,263,246', 'Capital': '69,210,567', 'Gastos administracion': '7,847,498', 'Gastos operacion': '237,380,091', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '32,187,204', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '253,093,284', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '3,052,280', 'Tipo de donante': 'Persona Física Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'INTERESES', 'Monto': '774,137'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'CUENTA CON VOLUNTARIOS', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '201,687', 'Conceptos Ejercidos': 'GASTOS FINANCIEROS'}, {'Monto': '7,049,671', 'Conceptos Ejercidos': 'GASTOS POR IVA'}, {'Monto': '229,570,922', 'Conceptos Ejercidos': 'COSTO EXISTENCIAL ORQUESTAS SINFONICAS ESPERANZA AZTECA'}, {'Monto': '557,811', 'Conceptos Ejercidos': 'IMPUESTO SOBRE LA RENTA'}]}, {'Donativos': []}], 'Actividades': [{'Actividades': [{'Actividad': 'Poner al alcance de niños y jovenes en situación de vulnerabilidad y exclusión una vía social, artística y educativa que ofrezca: Incremento de autoestima, Oportunidades, Aprendizaje, Comunicación con un lenguaje universal que es la música,entusiasmo personal, Bienestar familiar, Beneficios por la comunidad y Amor por México.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Acercar, enriquecer y ampliar el aprendizaje cultural de niños y jóvenes.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}, {'Actividad': 'Brindar una alternativa que desarrolle capacidades creativas, competitivas y productivas en niños y jóvenes, frente a la crisis económica, la drogadicción, la delincuencia y la pobreza cultural.', 'Número de Beneficiarios': '16000', 'Entidad Federativa': 'Nacional', 'Municipio': 'TODOS'}]}]}</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>{'Mision': 'Darles un hogar digno en el que se encuentren felices y amados', 'Vision': 'Concluir la obra para poder trasladarlas, y poderles dar mejores espacios y areas verdes para que tengan mas comodidad, y acoger a muchos mas ya que la sociedad lo necesita, ya que el actual es muy pequeño ya que es una casa prestada', 'Pagina web': 'N/A', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'FELISA SANCHEZ FERNANDEZ, MARTIN HERNANDEZ, FRANCISCO LOPEZ AGUILAR, VICTOR ALFONSO GARCIA HERNANDEZ.', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '3', 'Plantilla voluntariado': '6', 'Monto total plantilla laboral': '30,000', 'Activo': '3,998,689', 'Pasivo': '0', 'Capital': '3,998,689', 'Gastos administracion': '2,999', 'Gastos operacion': '432,572', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '2,015,203', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': 'MATERIALES PARA CONSTRUCCION', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MUEBLES Y ENSERES MENORES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': '', 'Efectivo ': '2,015,203', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': 'MATERIALES PARA CONSTRUCCION', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}, {'Especie ': 'MUEBLES Y ENSERES MENORES', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Pública Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'RIFAS', 'Monto': '0'}, {'Concepto': 'CUOTAS DE RECUPERACION', 'Monto': '47,526'}, {'Concepto': 'INTERESES BANCARIOS', 'Monto': '236'}, {'Concepto': 'REEMBOLSO POR CAJA', 'Monto': '1,227'}, {'Concepto': 'BAZAR', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'NO SE OTORGARON PERCEPCIONES', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '6,870', 'Conceptos Ejercidos': 'MANTENIMIENTO Y EQUIPO DE COMPUTO'}, {'Monto': '1,581,742', 'Conceptos Ejercidos': 'GASTOS POR OBRA CONSTRUCCION'}, {'Monto': '197,674', 'Conceptos Ejercidos': 'IVA ACREDITABLE'}, {'Monto': '214', 'Conceptos Ejercidos': 'FLETES Y ACARREOS'}, {'Monto': '30,000', 'Conceptos Ejercidos': 'SUELDOS A ASIMILADOS'}, {'Monto': '7,807', 'Conceptos Ejercidos': 'ALIMENTOS Y COMIDAS'}, {'Monto': '4,910', 'Conceptos Ejercidos': 'DIVERSOS'}, {'Monto': '138,489', 'Conceptos Ejercidos': 'MANTENIMIENTO E INSTALACION'}, {'Monto': '1,377', 'Conceptos Ejercidos': 'PAPELERIA Y UTILES'}, {'Monto': '2,999', 'Conceptos Ejercidos': 'GASTOS FINANCIEROS'}, {'Monto': '3,665', 'Conceptos Ejercidos': 'GAS'}, {'Monto': '2,159', 'Conceptos Ejercidos': 'SERVICIO TELEFONICO'}, {'Monto': '2,467', 'Conceptos Ejercidos': 'ENERGIA ELECTRICA'}, {'Monto': '5,478', 'Conceptos Ejercidos': 'OTROS'}, {'Monto': '0', 'Conceptos Ejercidos': 'PAPELERIA'}, {'Monto': '34,598', 'Conceptos Ejercidos': 'DESPENSA'}, {'Monto': '2,731', 'Conceptos Ejercidos': 'MEDICAMENTO Y BOTIQUIN'}, {'Monto': '117,512', 'Conceptos Ejercidos': 'ACTIVOS FIJOS MOBILIARIO Y EQUIPO'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'NO SE OTORGARON'}]}], 'Actividades': [{'Actividades': []}]}</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>{'Mision': '', 'Vision': '', 'Pagina web': '', 'Anio de autorizacion': '2012', 'Socios o Asociados': '', 'Rubros autorizados': ['H. Organizaciones Civiles y Fideicomisos de Apoyo Económico de Otras Donatarias Autorizadas.'], 'Plantilla laboral': '', 'Plantilla voluntariado': '', 'Monto total plantilla laboral': '0', 'Activo': '8,338', 'Pasivo': '45,000', 'Capital': '-36,662', 'Gastos administracion': '0', 'Gastos operacion': '3,732', 'Gastos representacion': '0', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '0', 'Tipo de donante': 'No aplica'}]}, {'OtrosIngresos': [{'Concepto': 'Ninguno', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'N/A', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': []}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'N/A'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'N/A', 'Número de Beneficiarios': '0', 'Entidad Federativa': 'Nacional', 'Municipio': 'N/A'}]}]}</t>
+          <t>{'Mision': 'Mejorar la calidad de vida de los ancianos en abandono y maltrato en Guadalajara y zona Metropolitana', 'Vision': 'Ser Una Organizacion Reconocida a nivel nacional por el excelente trato y servicio antencion que se le brinda a los ancianos', 'Pagina web': 'http://asunciondemariaseniorshome.keyrgs.com', 'Anio de autorizacion': '2013', 'Socios o Asociados': 'Jaime Suarez Valencia, Pdte. Felisa Sanchez Fernandez, Srio. Esteban Garcia Reyes, Escrutadores Victor Alfonso Garcia Hernandez y Juana Rodriguez Contreras', 'Rubros autorizados': ['A. Organizaciones Civiles y Fideicomisos Asistenciales.'], 'Plantilla laboral': '10', 'Plantilla voluntariado': '13', 'Monto total plantilla laboral': '166,797', 'Activo': '13,155,681', 'Pasivo': '433,466', 'Capital': '12,561,210', 'Gastos administracion': '1,403', 'Gastos operacion': '908,913', 'Gastos representacion': '27,482', 'Ingresos': [{'Ingresos': [{'Especie ': '', 'Efectivo ': '45,000', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': 'Medicamentos y Despensa por 56736', 'Efectivo ': '', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '30,000', 'Tipo de donante': 'Persona Moral Privada Nacional'}, {'Especie ': '', 'Efectivo ': '994,215', 'Tipo de donante': 'Persona Física Nacional'}, {'Especie ': '', 'Efectivo ': '56,000', 'Tipo de donante': 'Persona Moral Pública Nacional'}]}, {'OtrosIngresos': [{'Concepto': 'Ninguno', 'Monto': '0'}]}], 'Egresos': [{'Egresos': [{'Cargo ó Nombramiento': 'Ninguno', 'Total de percepciones netas': '0'}]}, {'MontosConceptos': [{'Monto': '0', 'Conceptos Ejercidos': 'Ninguno'}]}, {'Donativos': [{'Donativos': '0', 'Beneficiarios': 'Ninguno'}]}], 'Actividades': [{'Actividades': [{'Actividad': 'Estancia asilo de ancianos', 'Número de Beneficiarios': '120', 'Entidad Federativa': 'Jalisco', 'Municipio': 'varios'}]}]}</t>
         </is>
       </c>
     </row>

</xml_diff>